<commit_message>
added distance as text
</commit_message>
<xml_diff>
--- a/SmorgLocations.xlsx
+++ b/SmorgLocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrislim/Desktop/smorgasburgAR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A43EC6-6383-CF4A-9C31-963A379F0076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B4B895-DFEF-3C4F-A0A8-9C0121B2E482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{C9EA5B25-40FF-AA4B-B1CB-3FA029F03E5F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Location</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>3711 Halldale Ave</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F398EF5-1D43-0749-8363-0C6722135F3C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,6 +501,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>34.018956305811898</v>
+      </c>
+      <c r="D5">
+        <v>-118.28375294545</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>